<commit_message>
Auto stash before merge of "fix/teacher-login-v2" and "origin/fix/teacher-login-v2"
</commit_message>
<xml_diff>
--- a/rules/821.xlsx
+++ b/rules/821.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="24045" windowHeight="12255"/>
+    <workbookView windowHeight="17655"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -53,7 +53,7 @@
     <t>所在部门</t>
   </si>
   <si>
-    <t>张无忌</t>
+    <t>倚天剑</t>
   </si>
   <si>
     <t>其他</t>
@@ -62,10 +62,10 @@
     <t>男</t>
   </si>
   <si>
-    <t>大东区二O二小学</t>
+    <t>沈阳市8月底01分校</t>
   </si>
   <si>
-    <t>督导处</t>
+    <t>学校</t>
   </si>
 </sst>
 </file>
@@ -1286,8 +1286,8 @@
   <sheetPr/>
   <dimension ref="A1:H13"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="81" zoomScaleNormal="81" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView tabSelected="1" zoomScale="81" zoomScaleNormal="81" workbookViewId="0">
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.23333333333333" defaultRowHeight="14.25" outlineLevelCol="7"/>
@@ -1339,13 +1339,13 @@
         <v>8</v>
       </c>
       <c r="B3">
-        <v>13458964523</v>
+        <v>15647896523</v>
       </c>
       <c r="C3" s="8" t="s">
         <v>9</v>
       </c>
       <c r="D3">
-        <v>13458964523</v>
+        <v>15647896523</v>
       </c>
       <c r="E3" s="9">
         <v>29567</v>

</xml_diff>